<commit_message>
Update analysis scripts, fix Ligue 1 aliases, and update prediction data
</commit_message>
<xml_diff>
--- a/all stats/Serie_A_Stats.xlsx
+++ b/all stats/Serie_A_Stats.xlsx
@@ -46376,8 +46376,6 @@
           <t>Milan</t>
         </is>
       </c>
-      <c r="F351" t="inlineStr"/>
-      <c r="G351" t="inlineStr"/>
       <c r="H351" t="inlineStr">
         <is>
           <t>2</t>
@@ -66927,7 +66925,6 @@
           <t>Yael Trepy</t>
         </is>
       </c>
-      <c r="C513" t="inlineStr"/>
       <c r="D513" t="inlineStr">
         <is>
           <t>FW</t>
@@ -66938,8 +66935,6 @@
           <t>Cagliari</t>
         </is>
       </c>
-      <c r="F513" t="inlineStr"/>
-      <c r="G513" t="inlineStr"/>
       <c r="H513" t="inlineStr">
         <is>
           <t>2</t>

</xml_diff>